<commit_message>
update gerber files and clean up for production
</commit_message>
<xml_diff>
--- a/hardware/hcuduino_production_files/Rev1.0/BOM/BOM_PartType-hcuduino_r1.0.xlsx
+++ b/hardware/hcuduino_production_files/Rev1.0/BOM/BOM_PartType-hcuduino_r1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\hcu_hardware\hardware\zeleno_hcuduino\REV1.0\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7446C42-A897-4CD4-A0A7-A556AF0FEF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E487B986-1A5B-4BC0-A361-4044CE048086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{631B98C8-4DDF-465E-A055-94CF091B2472}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66ED291E-5F0A-46F0-AEF2-62900D51D654}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-hcuduino_r1.0" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B95BF89-269F-40A6-B4FE-AC4A6398C3D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{234799B9-D77D-495E-9C6C-549F398F5FB4}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>